<commit_message>
updated connection api backend
</commit_message>
<xml_diff>
--- a/KEPENGURUSAN KKNT SONGAN A.xlsx
+++ b/KEPENGURUSAN KKNT SONGAN A.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web-kkn-songana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC308A1-51C3-46ED-AB78-0853560036EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A310F8FF-3C46-468D-8EC4-D4B19427E834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2224CAEF-137C-4B11-B2EB-CF4771F525E5}"/>
+    <workbookView xWindow="28830" yWindow="45" windowWidth="20460" windowHeight="10770" xr2:uid="{2224CAEF-137C-4B11-B2EB-CF4771F525E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$B$1:$B$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="148">
   <si>
     <t>Indra Dwisaputra</t>
   </si>
@@ -301,16 +303,194 @@
   </si>
   <si>
     <t>IGedeTeguhBrahmastraWiradharma</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>andra.fahreza@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>ayu.laras@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>ashya.siva@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>yesi.citrayani@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>ayodhia@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>putrayasa.4@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>ayu.krisnayani@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>tia.pratiwi.2@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>st@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>andika.andara@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>rio.teguh@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>surya.ardi@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>gelgel.abdiutama@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>adith@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>ariana.2@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>yasana@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>dharma.sudana@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>zivi@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>indra.dwisaputra@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>varelly@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>gita.ariani@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>luluk.mukarromah@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>polanda@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>marini.arianti@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>teguh.brahmastra@undiksha.ac.id</t>
+  </si>
+  <si>
+    <t>$2b$12$KoV3VPI2X8HhW.zgC4U43O/Jd2hjhW5/2yk5N9G/bB/qk9qZxQ6um</t>
+  </si>
+  <si>
+    <t>$2b$12$cFG9H6klXJ7ARjA7w8u1/.NDl7ZbzHQ7esmN868OHt4YcrbxnMYCG</t>
+  </si>
+  <si>
+    <t>$2b$12$PmOmjSDpvUoLf5e6VOKk/e3948JYWIFIKR0Z/qEYEoYShGHcWDPri</t>
+  </si>
+  <si>
+    <t>$2b$12$BQB6ltNYq1/Ga8668xPBW..XdwgtXAH1qaryuNzoXw.TycOAMBvIq</t>
+  </si>
+  <si>
+    <t>$2b$12$FWq4UVoR15E/Nn4XDJjLve2Zz5LDjs1bU9lIjZJnvZJGlPaSSTfBO</t>
+  </si>
+  <si>
+    <t>$2b$12$vU61SGcNchzDvhlc7n1cPORsCi.c54jJnbeUbg8OtLvF7P/uMVSzq</t>
+  </si>
+  <si>
+    <t>$2b$12$4J8jjBSYolYxR56BDDD0VOollVbMaRosv660lHb6h0zfGx0cgB72.</t>
+  </si>
+  <si>
+    <t>$2b$12$4GCWrpEI3ahYV8QzbXZL7es7QaNxlth7VKsIfRPMvcgQ4noSbLdKG</t>
+  </si>
+  <si>
+    <t>$2b$12$uRMKGOSLXD2I7eVEdiuxbudzf0.DCD05HYzT0pf68b6ai7hDJQt5.</t>
+  </si>
+  <si>
+    <t>$2b$12$v0CeJuGQDORNZUlFwj1UQO8lDPH305qPSIQI/p/95g4/Y8l3ugTw.</t>
+  </si>
+  <si>
+    <t>$2b$12$2PJUcx5UEcak5wx1XF4LIefwiaXSfUse0NmI0f20fkVayXOjsBLr6</t>
+  </si>
+  <si>
+    <t>$2b$12$ljZiOjT02LbpDtlZ3kZUcu2xz5mT0uXybq2P8Rnb2EwE0FjNGYchO</t>
+  </si>
+  <si>
+    <t>$2b$12$2sOChFPSKNwXTfpegCtDZuX7FZBOwJNjD8I0hW8jrR2.o.G84H4DO</t>
+  </si>
+  <si>
+    <t>$2b$12$tHCqi6IMWWlSepz9Tckbb.fU8vskVfiSWIgOcgQhBP8Frrm/dAfG2</t>
+  </si>
+  <si>
+    <t>$2b$12$RIpEnsPNKEgkTJZ.EPkaJubHsNLKEhKD2rDapxC.DO015tgLWrW7G</t>
+  </si>
+  <si>
+    <t>$2b$12$3w/WjlxytCMuy4LClJDFqu/Jz5KI33RNAPyOG5oz3AZn9jgI5/DMu</t>
+  </si>
+  <si>
+    <t>$2b$12$Pqs3.KiVwd3dRSi3xllVaubHzuC.o7aTXviJCdf2B8ggwQVMe57Qe</t>
+  </si>
+  <si>
+    <t>$2b$12$.66sE85Z3n2R3V8YLxZ2C.7aZaY4g9KmWqBSIVkwu6w/JmW1Y6VOS</t>
+  </si>
+  <si>
+    <t>$2b$12$uLePz.aICTPUnwIwv00kNulWANfOH18i8wWsD5Q/pZjq.5MAySAxa</t>
+  </si>
+  <si>
+    <t>$2b$12$vONwoIamp0Zz1d1O1sP6LuuX48aLFBQRYY2gpyScDUARZXM881Geu</t>
+  </si>
+  <si>
+    <t>$2b$12$4yRe2jTAO799ncdj3D83vORrWbuZZ1BiT/E78wjbm3yoSoUp4FUMm</t>
+  </si>
+  <si>
+    <t>$2b$12$PCyjBNPRP3Z10fuw4BK1GuAiFTxbFTZW.slTY.mx48TsbSa2OpKkG</t>
+  </si>
+  <si>
+    <t>$2b$12$4MzHmKoPmq2mnPflY62lNOq46G8/GY1XEXrAQvpDZ68XHvB149Gka</t>
+  </si>
+  <si>
+    <t>$2b$12$iqsdpBLFuT.wuGShgTRyqO5X45zMZeCpDZEkbSWMkfdWIehuloS.a</t>
+  </si>
+  <si>
+    <t>$2b$12$VwPj/D0cS449EMenLwAVVewrcKW2YAAwhjxwiA1NJ5xnvFosw2Y8e</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>created_at</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,8 +516,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,24 +833,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E677CF-151B-46A2-B229-10751FC93875}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="125.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="69.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -685,8 +867,14 @@
       <c r="E1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -702,8 +890,17 @@
       <c r="E2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2257025021</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -719,8 +916,17 @@
       <c r="E3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2117051189</v>
+      </c>
+      <c r="H3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -736,8 +942,17 @@
       <c r="E4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2117041012</v>
+      </c>
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -753,8 +968,17 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2114101039</v>
+      </c>
+      <c r="H5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -770,8 +994,17 @@
       <c r="E6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2117041230</v>
+      </c>
+      <c r="H6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -787,8 +1020,17 @@
       <c r="E7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2114101147</v>
+      </c>
+      <c r="H7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -804,8 +1046,17 @@
       <c r="E8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1915081018</v>
+      </c>
+      <c r="H8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -821,8 +1072,17 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2257015032</v>
+      </c>
+      <c r="H9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -838,8 +1098,17 @@
       <c r="E10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2118011031</v>
+      </c>
+      <c r="H10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -855,8 +1124,17 @@
       <c r="E11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2113101017</v>
+      </c>
+      <c r="H11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -872,8 +1150,17 @@
       <c r="E12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2114101135</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -889,8 +1176,17 @@
       <c r="E13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2115091103</v>
+      </c>
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -906,8 +1202,17 @@
       <c r="E14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2115101014</v>
+      </c>
+      <c r="H14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -923,8 +1228,17 @@
       <c r="E15" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2117041222</v>
+      </c>
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -940,8 +1254,17 @@
       <c r="E16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2117041149</v>
+      </c>
+      <c r="H16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -957,8 +1280,17 @@
       <c r="E17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2117041176</v>
+      </c>
+      <c r="H17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -974,8 +1306,17 @@
       <c r="E18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2117041191</v>
+      </c>
+      <c r="H18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -991,8 +1332,17 @@
       <c r="E19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2114101056</v>
+      </c>
+      <c r="H19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1008,8 +1358,17 @@
       <c r="E20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2113091019</v>
+      </c>
+      <c r="H20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1025,8 +1384,17 @@
       <c r="E21" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2115091101</v>
+      </c>
+      <c r="H21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1042,8 +1410,17 @@
       <c r="E22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2117051019</v>
+      </c>
+      <c r="H22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1059,8 +1436,17 @@
       <c r="E23" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2117051120</v>
+      </c>
+      <c r="H23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1076,8 +1462,17 @@
       <c r="E24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2015051108</v>
+      </c>
+      <c r="H24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1093,8 +1488,17 @@
       <c r="E25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2117051196</v>
+      </c>
+      <c r="H25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1109,6 +1513,15 @@
       </c>
       <c r="E26" t="s">
         <v>90</v>
+      </c>
+      <c r="F26" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2117051239</v>
+      </c>
+      <c r="H26" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1120,4 +1533,471 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE7E1A3-9942-433A-A000-EACD36040BBD}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="69.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B26" xr:uid="{A7E677CF-151B-46A2-B229-10751FC93875}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>